<commit_message>
Set up diffusivity versus cutoff volatility plots
</commit_message>
<xml_diff>
--- a/Code/Timescale_Analysis/Equilibrium_Time_Data.xlsx
+++ b/Code/Timescale_Analysis/Equilibrium_Time_Data.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="14">
   <si>
     <t>water molec frac</t>
   </si>
@@ -24,17 +24,147 @@
     <t>Size (nm)</t>
   </si>
   <si>
-    <t>Equilibrium Time (hours)</t>
-  </si>
-  <si>
-    <t>Diffusivity (caculate as r^2 / tau)</t>
+    <t>k</t>
+  </si>
+  <si>
+    <t>T</t>
+  </si>
+  <si>
+    <t>K</t>
+  </si>
+  <si>
+    <t>m2 kg s-2 K-1</t>
+  </si>
+  <si>
+    <t>D (m2 s-1)</t>
+  </si>
+  <si>
+    <t>Diffusivity m2/s (caculate as r^2 / tau)</t>
+  </si>
+  <si>
+    <t>Calculate Diffusivity as a function of Temperature assuming same hydrodynamic radius</t>
+  </si>
+  <si>
+    <t>η (Pa s - kg m-1 s-1)</t>
+  </si>
+  <si>
+    <t>T (°C)</t>
+  </si>
+  <si>
+    <r>
+      <t>r</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>h</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> (nm)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Calculate r</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>h</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> (hydrodynamic radius) D and eta for dry particle at 298 K (Shiraiwa plot)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Equilibrium Time (</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>τ</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>mix</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>)</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>(hours)</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -47,6 +177,36 @@
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <vertAlign val="subscript"/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <vertAlign val="subscript"/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -149,7 +309,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -164,6 +324,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="11" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -171,6 +338,71 @@
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>657225</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>447675</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="Rectangle 1"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="657225" y="5133975"/>
+          <a:ext cx="6105525" cy="1257300"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="00B0F0"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -458,18 +690,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B1:H18"/>
+  <dimension ref="B1:H32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
+  <cols>
+    <col min="2" max="2" width="10.875" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="2:8" ht="15" thickBot="1"/>
-    <row r="2" spans="2:8" ht="15">
+    <row r="2" spans="2:8" ht="16.5">
       <c r="B2" s="1" t="s">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
@@ -630,7 +865,7 @@
     <row r="10" spans="2:8" ht="15" thickBot="1"/>
     <row r="11" spans="2:8" ht="15">
       <c r="B11" s="1" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
@@ -678,28 +913,28 @@
         <v>1</v>
       </c>
       <c r="C14" s="7">
-        <f>($B14*0.000000001)^2 / C5 * 100^2</f>
-        <v>5.2132207277656142E-10</v>
+        <f>($B14*0.000000001)^2 / (C5*3600)</f>
+        <v>1.4481168688237817E-17</v>
       </c>
       <c r="D14" s="7">
-        <f t="shared" ref="D14:H14" si="0">($B14*0.000000001)^2 / D5 * 100^2</f>
-        <v>7.4989501469794237E-10</v>
+        <f t="shared" ref="D14:H14" si="0">($B14*0.000000001)^2 / (D5*3600)</f>
+        <v>2.0830417074942842E-17</v>
       </c>
       <c r="E14" s="7">
         <f t="shared" si="0"/>
-        <v>1.0786858154972635E-9</v>
+        <v>2.9963494874923981E-17</v>
       </c>
       <c r="F14" s="7">
         <f t="shared" si="0"/>
-        <v>1.8609602182534147E-9</v>
+        <v>5.1693339395928182E-17</v>
       </c>
       <c r="G14" s="7">
         <f t="shared" si="0"/>
-        <v>1.6485627006094739E-8</v>
+        <v>4.5793408350263164E-16</v>
       </c>
       <c r="H14" s="8">
         <f t="shared" si="0"/>
-        <v>1.4384494665510154E-8</v>
+        <v>3.9956929626417093E-16</v>
       </c>
     </row>
     <row r="15" spans="2:8">
@@ -707,28 +942,28 @@
         <v>10</v>
       </c>
       <c r="C15" s="7">
-        <f t="shared" ref="C15:H15" si="1">($B15*0.000000001)^2 / C6 * 100^2</f>
-        <v>5.7092615641092986E-11</v>
+        <f t="shared" ref="C15:H15" si="1">($B15*0.000000001)^2 / (C6*3600)</f>
+        <v>1.5859059900303606E-18</v>
       </c>
       <c r="D15" s="7">
         <f t="shared" si="1"/>
-        <v>8.2124731041505849E-11</v>
+        <v>2.2812425289307179E-18</v>
       </c>
       <c r="E15" s="7">
         <f t="shared" si="1"/>
-        <v>1.0786846519354301E-10</v>
+        <v>2.9963462553761943E-18</v>
       </c>
       <c r="F15" s="7">
         <f t="shared" si="1"/>
-        <v>1.7782804383816938E-10</v>
+        <v>4.939667884393594E-18</v>
       </c>
       <c r="G15" s="7">
         <f t="shared" si="1"/>
-        <v>1.6485627006094737E-9</v>
+        <v>4.5793408350263154E-17</v>
       </c>
       <c r="H15" s="8">
         <f t="shared" si="1"/>
-        <v>1.3745421056610518E-9</v>
+        <v>3.8181725157251443E-17</v>
       </c>
     </row>
     <row r="16" spans="2:8">
@@ -736,28 +971,28 @@
         <v>100</v>
       </c>
       <c r="C16" s="7">
-        <f t="shared" ref="C16:H16" si="2">($B16*0.000000001)^2 / C7 * 100^2</f>
-        <v>8.7254705209978472E-11</v>
+        <f t="shared" ref="C16:H16" si="2">($B16*0.000000001)^2 / (C7*3600)</f>
+        <v>2.4237418113882906E-18</v>
       </c>
       <c r="D16" s="7">
         <f t="shared" si="2"/>
-        <v>1.2551177425954331E-10</v>
+        <v>3.4864381738762034E-18</v>
       </c>
       <c r="E16" s="7">
         <f t="shared" si="2"/>
-        <v>1.6485627006094738E-10</v>
+        <v>4.5793408350263162E-18</v>
       </c>
       <c r="F16" s="7">
         <f t="shared" si="2"/>
-        <v>2.7177531790917817E-10</v>
+        <v>7.5493143863660613E-18</v>
       </c>
       <c r="G16" s="7">
         <f t="shared" si="2"/>
-        <v>2.6366510313260514E-9</v>
+        <v>7.3240306425723637E-17</v>
       </c>
       <c r="H16" s="8">
         <f t="shared" si="2"/>
-        <v>2.3006064398575469E-9</v>
+        <v>6.3905734440487415E-17</v>
       </c>
     </row>
     <row r="17" spans="2:8">
@@ -765,28 +1000,28 @@
         <v>1000</v>
       </c>
       <c r="C17" s="7">
-        <f t="shared" ref="C17:H17" si="3">($B17*0.000000001)^2 / C8 * 100^2</f>
-        <v>9.7015794171291133E-11</v>
+        <f t="shared" ref="C17:H17" si="3">($B17*0.000000001)^2 / (C8*3600)</f>
+        <v>2.6948831714247537E-18</v>
       </c>
       <c r="D17" s="7">
         <f t="shared" si="3"/>
-        <v>1.395523439909459E-10</v>
+        <v>3.8764539997484969E-18</v>
       </c>
       <c r="E17" s="7">
         <f t="shared" si="3"/>
-        <v>1.8329823172195866E-10</v>
+        <v>5.0916175478321849E-18</v>
       </c>
       <c r="F17" s="7">
         <f t="shared" si="3"/>
-        <v>3.0217779537124066E-10</v>
+        <v>8.3938276492011291E-18</v>
       </c>
       <c r="G17" s="7">
         <f t="shared" si="3"/>
-        <v>2.9316056404092534E-9</v>
+        <v>8.143349001136815E-17</v>
       </c>
       <c r="H17" s="8">
         <f t="shared" si="3"/>
-        <v>2.444318426250025E-9</v>
+        <v>6.7897734062500695E-17</v>
       </c>
     </row>
     <row r="18" spans="2:8" ht="15" thickBot="1">
@@ -794,32 +1029,163 @@
         <v>10000</v>
       </c>
       <c r="C18" s="12">
-        <f t="shared" ref="C18:H18" si="4">($B18*0.000000001)^2 / C9 * 100^2</f>
-        <v>1.9474841426103693E-10</v>
+        <f t="shared" ref="C18:H18" si="4">($B18*0.000000001)^2 / (C9*3600)</f>
+        <v>5.4096781739176922E-18</v>
       </c>
       <c r="D18" s="12">
         <f t="shared" si="4"/>
-        <v>2.8013558562344179E-10</v>
+        <v>7.7815440450956048E-18</v>
       </c>
       <c r="E18" s="12">
         <f t="shared" si="4"/>
-        <v>3.8505820154716385E-10</v>
+        <v>1.0696061154087887E-17</v>
       </c>
       <c r="F18" s="12">
         <f t="shared" si="4"/>
-        <v>6.3479166137673634E-10</v>
+        <v>1.7633101704909342E-17</v>
       </c>
       <c r="G18" s="12">
         <f t="shared" si="4"/>
-        <v>5.1348409226282187E-9</v>
+        <v>1.4263447007300607E-16</v>
       </c>
       <c r="H18" s="13">
         <f t="shared" si="4"/>
-        <v>4.480387105445911E-9</v>
+        <v>1.2445519737349753E-16</v>
+      </c>
+    </row>
+    <row r="20" spans="2:8">
+      <c r="B20" t="s">
+        <v>2</v>
+      </c>
+      <c r="C20" s="14">
+        <v>1.3800000000000001E-23</v>
+      </c>
+      <c r="D20" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="2:8">
+      <c r="B21" t="s">
+        <v>3</v>
+      </c>
+      <c r="C21">
+        <v>298</v>
+      </c>
+      <c r="D21" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="2:8" ht="16.5">
+      <c r="B23" s="15" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="24" spans="2:8" ht="28.5">
+      <c r="B24" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="C24" s="14">
+        <f>D31</f>
+        <v>7500000</v>
+      </c>
+    </row>
+    <row r="25" spans="2:8">
+      <c r="B25" t="s">
+        <v>6</v>
+      </c>
+      <c r="C25" s="14">
+        <f>C18</f>
+        <v>5.4096781739176922E-18</v>
+      </c>
+    </row>
+    <row r="26" spans="2:8" ht="16.5">
+      <c r="B26" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="C26" s="18">
+        <f>C20*C21/C25/6/PI()/C24*1000000000</f>
+        <v>5.3772661755803128E-3</v>
+      </c>
+    </row>
+    <row r="28" spans="2:8" ht="15">
+      <c r="B28" s="15" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="30" spans="2:8">
+      <c r="B30" t="s">
+        <v>10</v>
+      </c>
+      <c r="C30">
+        <v>0</v>
+      </c>
+      <c r="D30">
+        <v>25</v>
+      </c>
+      <c r="E30">
+        <v>50</v>
+      </c>
+      <c r="F30">
+        <v>100</v>
+      </c>
+      <c r="G30">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="31" spans="2:8" ht="28.5">
+      <c r="B31" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="C31" s="14">
+        <v>10000000</v>
+      </c>
+      <c r="D31" s="14">
+        <v>7500000</v>
+      </c>
+      <c r="E31" s="14">
+        <v>5000000</v>
+      </c>
+      <c r="F31" s="14">
+        <v>0.1</v>
+      </c>
+      <c r="G31" s="14">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="32" spans="2:8">
+      <c r="B32" t="s">
+        <v>6</v>
+      </c>
+      <c r="C32" s="14">
+        <f>$C$20*(C30+273)/6/PI()/C31/($C$26/1000000000)</f>
+        <v>3.7168845842605626E-18</v>
+      </c>
+      <c r="D32" s="14">
+        <f t="shared" ref="D32:G32" si="5">$C$20*(D30+273)/6/PI()/D31/($C$26/1000000000)</f>
+        <v>5.4096781739176937E-18</v>
+      </c>
+      <c r="E32" s="14">
+        <f t="shared" si="5"/>
+        <v>8.7952653532319544E-18</v>
+      </c>
+      <c r="F32" s="14">
+        <f t="shared" si="5"/>
+        <v>5.0783807689713913E-10</v>
+      </c>
+      <c r="G32" s="14">
+        <f t="shared" si="5"/>
+        <v>5.7591288613268068E-9</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <drawing r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
+  <oleObjects>
+    <oleObject progId="Equation.3" shapeId="1025" r:id="rId3"/>
+    <oleObject progId="Equation.3" shapeId="1026" r:id="rId4"/>
+  </oleObjects>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Done making plots Likely there is an error in the size dependnece of X
</commit_message>
<xml_diff>
--- a/Code/Timescale_Analysis/Equilibrium_Time_Data.xlsx
+++ b/Code/Timescale_Analysis/Equilibrium_Time_Data.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="20">
   <si>
     <t>water molec frac</t>
   </si>
@@ -37,12 +37,6 @@
   </si>
   <si>
     <t>D (m2 s-1)</t>
-  </si>
-  <si>
-    <t>Diffusivity m2/s (caculate as r^2 / tau)</t>
-  </si>
-  <si>
-    <t>Calculate Diffusivity as a function of Temperature assuming same hydrodynamic radius</t>
   </si>
   <si>
     <t>η (Pa s - kg m-1 s-1)</t>
@@ -103,8 +97,26 @@
     </r>
   </si>
   <si>
+    <t>Diffusivity m2/s (caculate as r^2 / pi^2 / tau)</t>
+  </si>
+  <si>
+    <t>minD</t>
+  </si>
+  <si>
+    <t>maxD</t>
+  </si>
+  <si>
+    <t>Water Mole Frac</t>
+  </si>
+  <si>
+    <t>T (deg C)</t>
+  </si>
+  <si>
+    <t>Digitize Viscosity (Pa s) as a Function of Temperature and Water</t>
+  </si>
+  <si>
     <r>
-      <t>Equilibrium Time (</t>
+      <t>Digitize Equilibrium Time (</t>
     </r>
     <r>
       <rPr>
@@ -158,6 +170,12 @@
       </rPr>
       <t>(hours)</t>
     </r>
+  </si>
+  <si>
+    <t>Calculate Diffusivity (m2 s-1) as a Function of Temperature and Water</t>
+  </si>
+  <si>
+    <t>Calculate Dry Diffusivity as a function of Temperature assuming same hydrodynamic radius</t>
   </si>
 </sst>
 </file>
@@ -351,7 +369,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>447675</xdr:colOff>
+      <xdr:colOff>657225</xdr:colOff>
       <xdr:row>32</xdr:row>
       <xdr:rowOff>104775</xdr:rowOff>
     </xdr:to>
@@ -362,8 +380,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="657225" y="5133975"/>
-          <a:ext cx="6105525" cy="1257300"/>
+          <a:off x="657225" y="5143500"/>
+          <a:ext cx="6315075" cy="1257300"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -690,10 +708,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B1:H32"/>
+  <dimension ref="B1:K106"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B35" sqref="B35"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K50" sqref="K50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -704,7 +722,7 @@
     <row r="1" spans="2:8" ht="15" thickBot="1"/>
     <row r="2" spans="2:8" ht="16.5">
       <c r="B2" s="1" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
@@ -865,7 +883,7 @@
     <row r="10" spans="2:8" ht="15" thickBot="1"/>
     <row r="11" spans="2:8" ht="15">
       <c r="B11" s="1" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
@@ -913,28 +931,28 @@
         <v>1</v>
       </c>
       <c r="C14" s="7">
-        <f>($B14*0.000000001)^2 / (C5*3600)</f>
-        <v>1.4481168688237817E-17</v>
+        <f>($B14*0.000000001/2)^2 / (C5*3600) / (PI()^2)</f>
+        <v>3.668122880041539E-19</v>
       </c>
       <c r="D14" s="7">
-        <f t="shared" ref="D14:H14" si="0">($B14*0.000000001)^2 / (D5*3600)</f>
-        <v>2.0830417074942842E-17</v>
+        <f t="shared" ref="D14:H14" si="0">($B14*0.000000001/2)^2 / (D5*3600) / (PI()^2)</f>
+        <v>5.2764062844919309E-19</v>
       </c>
       <c r="E14" s="7">
         <f t="shared" si="0"/>
-        <v>2.9963494874923981E-17</v>
+        <v>7.5898419169710487E-19</v>
       </c>
       <c r="F14" s="7">
         <f t="shared" si="0"/>
-        <v>5.1693339395928182E-17</v>
+        <v>1.3094075835051334E-18</v>
       </c>
       <c r="G14" s="7">
         <f t="shared" si="0"/>
-        <v>4.5793408350263164E-16</v>
+        <v>1.1599605842663946E-17</v>
       </c>
       <c r="H14" s="8">
         <f t="shared" si="0"/>
-        <v>3.9956929626417093E-16</v>
+        <v>1.0121208511155434E-17</v>
       </c>
     </row>
     <row r="15" spans="2:8">
@@ -942,28 +960,28 @@
         <v>10</v>
       </c>
       <c r="C15" s="7">
-        <f t="shared" ref="C15:H15" si="1">($B15*0.000000001)^2 / (C6*3600)</f>
-        <v>1.5859059900303606E-18</v>
+        <f t="shared" ref="C15:H15" si="1">($B15*0.000000001/2)^2 / (C6*3600) / (PI()^2)</f>
+        <v>4.0171468013837419E-20</v>
       </c>
       <c r="D15" s="7">
         <f t="shared" si="1"/>
-        <v>2.2812425289307179E-18</v>
+        <v>5.7784548301625085E-20</v>
       </c>
       <c r="E15" s="7">
         <f t="shared" si="1"/>
-        <v>2.9963462553761943E-18</v>
+        <v>7.5898337299250624E-20</v>
       </c>
       <c r="F15" s="7">
         <f t="shared" si="1"/>
-        <v>4.939667884393594E-18</v>
+        <v>1.2512324921170036E-19</v>
       </c>
       <c r="G15" s="7">
         <f t="shared" si="1"/>
-        <v>4.5793408350263154E-17</v>
+        <v>1.1599605842663942E-18</v>
       </c>
       <c r="H15" s="8">
         <f t="shared" si="1"/>
-        <v>3.8181725157251443E-17</v>
+        <v>9.671543966097855E-19</v>
       </c>
     </row>
     <row r="16" spans="2:8">
@@ -971,89 +989,103 @@
         <v>100</v>
       </c>
       <c r="C16" s="7">
-        <f t="shared" ref="C16:H16" si="2">($B16*0.000000001)^2 / (C7*3600)</f>
-        <v>2.4237418113882906E-18</v>
+        <f t="shared" ref="C16:H16" si="2">($B16*0.000000001/2)^2 / (C7*3600) / (PI()^2)</f>
+        <v>6.1394097293321348E-20</v>
       </c>
       <c r="D16" s="7">
         <f t="shared" si="2"/>
-        <v>3.4864381738762034E-18</v>
+        <v>8.8312510618241895E-20</v>
       </c>
       <c r="E16" s="7">
         <f t="shared" si="2"/>
-        <v>4.5793408350263162E-18</v>
+        <v>1.1599605842663946E-19</v>
       </c>
       <c r="F16" s="7">
         <f t="shared" si="2"/>
-        <v>7.5493143863660613E-18</v>
+        <v>1.9122636732868457E-19</v>
       </c>
       <c r="G16" s="7">
         <f t="shared" si="2"/>
-        <v>7.3240306425723637E-17</v>
+        <v>1.8551986343454592E-18</v>
       </c>
       <c r="H16" s="8">
         <f t="shared" si="2"/>
-        <v>6.3905734440487415E-17</v>
-      </c>
-    </row>
-    <row r="17" spans="2:8">
+        <v>1.6187511637607738E-18</v>
+      </c>
+    </row>
+    <row r="17" spans="2:11">
       <c r="B17" s="4">
         <v>1000</v>
       </c>
       <c r="C17" s="7">
-        <f t="shared" ref="C17:H17" si="3">($B17*0.000000001)^2 / (C8*3600)</f>
-        <v>2.6948831714247537E-18</v>
+        <f t="shared" ref="C17:H17" si="3">($B17*0.000000001/2)^2 / (C8*3600) / (PI()^2)</f>
+        <v>6.8262188176643274E-20</v>
       </c>
       <c r="D17" s="7">
         <f t="shared" si="3"/>
-        <v>3.8764539997484969E-18</v>
+        <v>9.8191726897398061E-20</v>
       </c>
       <c r="E17" s="7">
         <f t="shared" si="3"/>
-        <v>5.0916175478321849E-18</v>
+        <v>1.2897217915011358E-19</v>
       </c>
       <c r="F17" s="7">
         <f t="shared" si="3"/>
-        <v>8.3938276492011291E-18</v>
+        <v>2.1261813817671E-19</v>
       </c>
       <c r="G17" s="7">
         <f t="shared" si="3"/>
-        <v>8.143349001136815E-17</v>
+        <v>2.0627343990195779E-18</v>
       </c>
       <c r="H17" s="8">
         <f t="shared" si="3"/>
-        <v>6.7897734062500695E-17</v>
-      </c>
-    </row>
-    <row r="18" spans="2:8" ht="15" thickBot="1">
+        <v>1.7198696954613114E-18</v>
+      </c>
+      <c r="J17" t="s">
+        <v>12</v>
+      </c>
+      <c r="K17" s="14">
+        <f>MIN(C14:H18)</f>
+        <v>4.0171468013837419E-20</v>
+      </c>
+    </row>
+    <row r="18" spans="2:11" ht="15" thickBot="1">
       <c r="B18" s="9">
         <v>10000</v>
       </c>
       <c r="C18" s="12">
-        <f t="shared" ref="C18:H18" si="4">($B18*0.000000001)^2 / (C9*3600)</f>
-        <v>5.4096781739176922E-18</v>
+        <f t="shared" ref="C18:H18" si="4">($B18*0.000000001/2)^2 / (C9*3600) / (PI()^2)</f>
+        <v>1.3702874892636524E-19</v>
       </c>
       <c r="D18" s="12">
         <f t="shared" si="4"/>
-        <v>7.7815440450956048E-18</v>
+        <v>1.9710881330351793E-19</v>
       </c>
       <c r="E18" s="12">
         <f t="shared" si="4"/>
-        <v>1.0696061154087887E-17</v>
+        <v>2.7093439411075354E-19</v>
       </c>
       <c r="F18" s="12">
         <f t="shared" si="4"/>
-        <v>1.7633101704909342E-17</v>
+        <v>4.4665168400678466E-19</v>
       </c>
       <c r="G18" s="12">
         <f t="shared" si="4"/>
-        <v>1.4263447007300607E-16</v>
+        <v>3.6129733339986452E-18</v>
       </c>
       <c r="H18" s="13">
         <f t="shared" si="4"/>
-        <v>1.2445519737349753E-16</v>
-      </c>
-    </row>
-    <row r="20" spans="2:8">
+        <v>3.1524869770808846E-18</v>
+      </c>
+      <c r="J18" t="s">
+        <v>13</v>
+      </c>
+      <c r="K18" s="14">
+        <f>MAX(C14:H18)</f>
+        <v>1.1599605842663946E-17</v>
+      </c>
+    </row>
+    <row r="20" spans="2:11">
       <c r="B20" t="s">
         <v>2</v>
       </c>
@@ -1064,7 +1096,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="2:8">
+    <row r="21" spans="2:11">
       <c r="B21" t="s">
         <v>3</v>
       </c>
@@ -1075,46 +1107,46 @@
         <v>4</v>
       </c>
     </row>
-    <row r="23" spans="2:8" ht="16.5">
+    <row r="23" spans="2:11" ht="16.5">
       <c r="B23" s="15" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="24" spans="2:8" ht="28.5">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="24" spans="2:11" ht="28.5">
       <c r="B24" s="16" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C24" s="14">
         <f>D31</f>
         <v>7500000</v>
       </c>
     </row>
-    <row r="25" spans="2:8">
+    <row r="25" spans="2:11">
       <c r="B25" t="s">
         <v>6</v>
       </c>
       <c r="C25" s="14">
         <f>C18</f>
-        <v>5.4096781739176922E-18</v>
-      </c>
-    </row>
-    <row r="26" spans="2:8" ht="16.5">
+        <v>1.3702874892636524E-19</v>
+      </c>
+    </row>
+    <row r="26" spans="2:11" ht="16.5">
       <c r="B26" s="17" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C26" s="18">
         <f>C20*C21/C25/6/PI()/C24*1000000000</f>
-        <v>5.3772661755803128E-3</v>
-      </c>
-    </row>
-    <row r="28" spans="2:8" ht="15">
+        <v>0.21228595964934563</v>
+      </c>
+    </row>
+    <row r="28" spans="2:11" ht="15">
       <c r="B28" s="15" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="30" spans="2:11">
+      <c r="B30" t="s">
         <v>8</v>
-      </c>
-    </row>
-    <row r="30" spans="2:8">
-      <c r="B30" t="s">
-        <v>10</v>
       </c>
       <c r="C30">
         <v>0</v>
@@ -1132,9 +1164,9 @@
         <v>150</v>
       </c>
     </row>
-    <row r="31" spans="2:8" ht="28.5">
+    <row r="31" spans="2:11" ht="28.5">
       <c r="B31" s="16" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C31" s="14">
         <v>10000000</v>
@@ -1152,32 +1184,786 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="32" spans="2:8">
+    <row r="32" spans="2:11">
       <c r="B32" t="s">
         <v>6</v>
       </c>
       <c r="C32" s="14">
         <f>$C$20*(C30+273)/6/PI()/C31/($C$26/1000000000)</f>
-        <v>3.7168845842605626E-18</v>
+        <v>9.4149786384809678E-20</v>
       </c>
       <c r="D32" s="14">
         <f t="shared" ref="D32:G32" si="5">$C$20*(D30+273)/6/PI()/D31/($C$26/1000000000)</f>
-        <v>5.4096781739176937E-18</v>
+        <v>1.3702874892636524E-19</v>
       </c>
       <c r="E32" s="14">
         <f t="shared" si="5"/>
-        <v>8.7952653532319544E-18</v>
+        <v>2.2278667400947639E-19</v>
       </c>
       <c r="F32" s="14">
         <f t="shared" si="5"/>
-        <v>5.0783807689713913E-10</v>
+        <v>1.286368876246667E-11</v>
       </c>
       <c r="G32" s="14">
         <f t="shared" si="5"/>
-        <v>5.7591288613268068E-9</v>
-      </c>
+        <v>1.4588043824459524E-10</v>
+      </c>
+    </row>
+    <row r="35" spans="2:8" ht="15" thickBot="1"/>
+    <row r="36" spans="2:8" ht="15">
+      <c r="B36" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C36" s="2"/>
+      <c r="D36" s="2"/>
+      <c r="E36" s="2"/>
+      <c r="F36" s="2"/>
+      <c r="G36" s="2"/>
+      <c r="H36" s="3"/>
+    </row>
+    <row r="37" spans="2:8">
+      <c r="B37" s="4"/>
+      <c r="C37" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D37" s="5"/>
+      <c r="E37" s="5"/>
+      <c r="F37" s="5"/>
+      <c r="G37" s="5"/>
+      <c r="H37" s="6"/>
+    </row>
+    <row r="38" spans="2:8">
+      <c r="B38" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C38" s="5">
+        <v>0</v>
+      </c>
+      <c r="D38" s="5">
+        <v>0.25</v>
+      </c>
+      <c r="E38" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="F38" s="5">
+        <v>0.75</v>
+      </c>
+      <c r="G38" s="5">
+        <v>0.9</v>
+      </c>
+      <c r="H38" s="6">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="39" spans="2:8">
+      <c r="B39" s="4">
+        <v>0</v>
+      </c>
+      <c r="C39" s="7">
+        <v>8554670</v>
+      </c>
+      <c r="D39" s="7">
+        <v>5568810</v>
+      </c>
+      <c r="E39" s="7">
+        <v>8554670</v>
+      </c>
+      <c r="F39" s="7">
+        <v>1867180</v>
+      </c>
+      <c r="G39" s="5">
+        <v>275853</v>
+      </c>
+      <c r="H39" s="6">
+        <v>286832</v>
+      </c>
+    </row>
+    <row r="40" spans="2:8">
+      <c r="B40" s="4">
+        <v>5</v>
+      </c>
+      <c r="C40" s="7">
+        <v>8227240</v>
+      </c>
+      <c r="D40" s="7">
+        <v>5568810</v>
+      </c>
+      <c r="E40" s="7">
+        <v>7609500</v>
+      </c>
+      <c r="F40" s="7">
+        <v>1941490</v>
+      </c>
+      <c r="G40" s="5">
+        <v>255141</v>
+      </c>
+      <c r="H40" s="6">
+        <v>286832</v>
+      </c>
+    </row>
+    <row r="41" spans="2:8">
+      <c r="B41" s="4">
+        <v>10</v>
+      </c>
+      <c r="C41" s="7">
+        <v>7318240</v>
+      </c>
+      <c r="D41" s="7">
+        <v>5568810</v>
+      </c>
+      <c r="E41" s="7">
+        <v>7038140</v>
+      </c>
+      <c r="F41" s="7">
+        <v>1795710</v>
+      </c>
+      <c r="G41" s="5">
+        <v>255141</v>
+      </c>
+      <c r="H41" s="6">
+        <v>275853</v>
+      </c>
+    </row>
+    <row r="42" spans="2:8">
+      <c r="B42" s="4">
+        <v>20</v>
+      </c>
+      <c r="C42" s="7">
+        <v>5355670</v>
+      </c>
+      <c r="D42" s="7">
+        <v>4406240</v>
+      </c>
+      <c r="E42" s="7">
+        <v>4953540</v>
+      </c>
+      <c r="F42" s="7">
+        <v>1536180</v>
+      </c>
+      <c r="G42" s="5">
+        <v>226951</v>
+      </c>
+      <c r="H42" s="6">
+        <v>265295</v>
+      </c>
+    </row>
+    <row r="43" spans="2:8">
+      <c r="B43" s="4">
+        <v>30</v>
+      </c>
+      <c r="C43" s="7">
+        <v>5150680</v>
+      </c>
+      <c r="D43" s="7">
+        <v>4237590</v>
+      </c>
+      <c r="E43" s="7">
+        <v>3224590</v>
+      </c>
+      <c r="F43" s="7">
+        <v>1420830</v>
+      </c>
+      <c r="G43" s="5">
+        <v>218264</v>
+      </c>
+      <c r="H43" s="6">
+        <v>226951</v>
+      </c>
+    </row>
+    <row r="44" spans="2:8">
+      <c r="B44" s="4">
+        <v>40</v>
+      </c>
+      <c r="C44" s="7">
+        <v>4237590</v>
+      </c>
+      <c r="D44" s="7">
+        <v>3919410</v>
+      </c>
+      <c r="E44" s="7">
+        <v>1660880</v>
+      </c>
+      <c r="F44" s="5">
+        <v>855467</v>
+      </c>
+      <c r="G44" s="5">
+        <v>172698</v>
+      </c>
+      <c r="H44" s="6">
+        <v>186718</v>
+      </c>
+    </row>
+    <row r="45" spans="2:8">
+      <c r="B45" s="4">
+        <v>50</v>
+      </c>
+      <c r="C45" s="7">
+        <v>2453750</v>
+      </c>
+      <c r="D45" s="7">
+        <v>1795710</v>
+      </c>
+      <c r="E45" s="5">
+        <v>286832</v>
+      </c>
+      <c r="F45" s="5">
+        <v>650968</v>
+      </c>
+      <c r="G45" s="5">
+        <v>136645</v>
+      </c>
+      <c r="H45" s="6">
+        <v>159731</v>
+      </c>
+    </row>
+    <row r="46" spans="2:8">
+      <c r="B46" s="4">
+        <v>60</v>
+      </c>
+      <c r="C46" s="5">
+        <v>924915</v>
+      </c>
+      <c r="D46" s="5">
+        <v>889514</v>
+      </c>
+      <c r="E46" s="5">
+        <v>626052</v>
+      </c>
+      <c r="F46" s="5">
+        <v>255141</v>
+      </c>
+      <c r="G46" s="5">
+        <v>100000</v>
+      </c>
+      <c r="H46" s="6">
+        <v>126385</v>
+      </c>
+    </row>
+    <row r="47" spans="2:8">
+      <c r="B47" s="4">
+        <v>70</v>
+      </c>
+      <c r="C47" s="5">
+        <v>42375.9</v>
+      </c>
+      <c r="D47" s="5">
+        <v>391941</v>
+      </c>
+      <c r="E47" s="5">
+        <v>265295</v>
+      </c>
+      <c r="F47" s="5">
+        <v>45816</v>
+      </c>
+      <c r="G47" s="5">
+        <v>3769.39</v>
+      </c>
+      <c r="H47" s="6">
+        <v>6768.75</v>
+      </c>
+    </row>
+    <row r="48" spans="2:8">
+      <c r="B48" s="4">
+        <v>80</v>
+      </c>
+      <c r="C48" s="5">
+        <v>5.1506800000000004</v>
+      </c>
+      <c r="D48" s="5">
+        <v>121547</v>
+      </c>
+      <c r="E48" s="5">
+        <v>60208.9</v>
+      </c>
+      <c r="F48" s="5">
+        <v>961.72500000000002</v>
+      </c>
+      <c r="G48" s="5">
+        <v>31.011700000000001</v>
+      </c>
+      <c r="H48" s="6">
+        <v>376.93900000000002</v>
+      </c>
+    </row>
+    <row r="49" spans="2:9" ht="15" thickBot="1">
+      <c r="B49" s="9">
+        <v>90</v>
+      </c>
+      <c r="C49" s="10">
+        <v>1.08118</v>
+      </c>
+      <c r="D49" s="10">
+        <v>2359.83</v>
+      </c>
+      <c r="E49" s="10">
+        <v>1867.18</v>
+      </c>
+      <c r="F49" s="10">
+        <v>0.79123399999999999</v>
+      </c>
+      <c r="G49" s="10">
+        <v>0.1</v>
+      </c>
+      <c r="H49" s="11">
+        <v>0.15973100000000001</v>
+      </c>
+    </row>
+    <row r="50" spans="2:9" ht="15" thickBot="1">
+      <c r="B50" s="14"/>
+      <c r="F50" s="14"/>
+      <c r="G50" s="14"/>
+      <c r="H50" s="14"/>
+      <c r="I50" s="14"/>
+    </row>
+    <row r="51" spans="2:9" ht="15">
+      <c r="B51" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C51" s="2"/>
+      <c r="D51" s="2"/>
+      <c r="E51" s="2"/>
+      <c r="F51" s="2"/>
+      <c r="G51" s="2"/>
+      <c r="H51" s="3"/>
+    </row>
+    <row r="52" spans="2:9">
+      <c r="B52" s="4"/>
+      <c r="C52" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D52" s="5"/>
+      <c r="E52" s="5"/>
+      <c r="F52" s="5"/>
+      <c r="G52" s="5"/>
+      <c r="H52" s="6"/>
+    </row>
+    <row r="53" spans="2:9">
+      <c r="B53" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C53" s="5">
+        <v>0</v>
+      </c>
+      <c r="D53" s="5">
+        <v>0.25</v>
+      </c>
+      <c r="E53" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="F53" s="5">
+        <v>0.75</v>
+      </c>
+      <c r="G53" s="5">
+        <v>0.9</v>
+      </c>
+      <c r="H53" s="6">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="54" spans="2:9">
+      <c r="B54" s="4">
+        <v>0</v>
+      </c>
+      <c r="C54" s="7">
+        <f>$C$20*($B54+273)/6/PI()/C39/($C$26/1000000000)</f>
+        <v>1.1005659643774648E-19</v>
+      </c>
+      <c r="D54" s="7">
+        <f t="shared" ref="D54:H54" si="6">$C$20*($B54+273)/6/PI()/D39/($C$26/1000000000)</f>
+        <v>1.6906625721619102E-19</v>
+      </c>
+      <c r="E54" s="7">
+        <f t="shared" si="6"/>
+        <v>1.1005659643774648E-19</v>
+      </c>
+      <c r="F54" s="7">
+        <f t="shared" si="6"/>
+        <v>5.0423519095539618E-19</v>
+      </c>
+      <c r="G54" s="7">
+        <f t="shared" si="6"/>
+        <v>3.4130419602037921E-18</v>
+      </c>
+      <c r="H54" s="8">
+        <f t="shared" si="6"/>
+        <v>3.2824017677528889E-18</v>
+      </c>
+    </row>
+    <row r="55" spans="2:9">
+      <c r="B55" s="4">
+        <v>5</v>
+      </c>
+      <c r="C55" s="7">
+        <f t="shared" ref="C55:H55" si="7">$C$20*($B55+273)/6/PI()/C40/($C$26/1000000000)</f>
+        <v>1.1653256918091916E-19</v>
+      </c>
+      <c r="D55" s="7">
+        <f t="shared" si="7"/>
+        <v>1.7216270881355716E-19</v>
+      </c>
+      <c r="E55" s="7">
+        <f t="shared" si="7"/>
+        <v>1.2599269524515739E-19</v>
+      </c>
+      <c r="F55" s="7">
+        <f t="shared" si="7"/>
+        <v>4.9381733332029787E-19</v>
+      </c>
+      <c r="G55" s="7">
+        <f t="shared" si="7"/>
+        <v>3.7576924699206523E-18</v>
+      </c>
+      <c r="H55" s="8">
+        <f t="shared" si="7"/>
+        <v>3.3425190162465315E-18</v>
+      </c>
+    </row>
+    <row r="56" spans="2:9">
+      <c r="B56" s="4">
+        <v>10</v>
+      </c>
+      <c r="C56" s="7">
+        <f t="shared" ref="C56:H56" si="8">$C$20*($B56+273)/6/PI()/C41/($C$26/1000000000)</f>
+        <v>1.3336334488728904E-19</v>
+      </c>
+      <c r="D56" s="7">
+        <f t="shared" si="8"/>
+        <v>1.7525916041092333E-19</v>
+      </c>
+      <c r="E56" s="7">
+        <f t="shared" si="8"/>
+        <v>1.3867086546842689E-19</v>
+      </c>
+      <c r="F56" s="7">
+        <f t="shared" si="8"/>
+        <v>5.4350923316568599E-19</v>
+      </c>
+      <c r="G56" s="7">
+        <f t="shared" si="8"/>
+        <v>3.8252768668616721E-18</v>
+      </c>
+      <c r="H56" s="8">
+        <f t="shared" si="8"/>
+        <v>3.5380618122259101E-18</v>
+      </c>
+    </row>
+    <row r="57" spans="2:9">
+      <c r="B57" s="4">
+        <v>20</v>
+      </c>
+      <c r="C57" s="7">
+        <f t="shared" ref="C57:H57" si="9">$C$20*($B57+273)/6/PI()/C42/($C$26/1000000000)</f>
+        <v>1.8867332496733574E-19</v>
+      </c>
+      <c r="D57" s="7">
+        <f t="shared" si="9"/>
+        <v>2.2932751423613125E-19</v>
+      </c>
+      <c r="E57" s="7">
+        <f t="shared" si="9"/>
+        <v>2.0398988729833835E-19</v>
+      </c>
+      <c r="F57" s="7">
+        <f t="shared" si="9"/>
+        <v>6.57782334314866E-19</v>
+      </c>
+      <c r="G57" s="7">
+        <f t="shared" si="9"/>
+        <v>4.4523798808016312E-18</v>
+      </c>
+      <c r="H57" s="8">
+        <f t="shared" si="9"/>
+        <v>3.808862083069077E-18</v>
+      </c>
+    </row>
+    <row r="58" spans="2:9">
+      <c r="B58" s="4">
+        <v>30</v>
+      </c>
+      <c r="C58" s="7">
+        <f t="shared" ref="C58:H58" si="10">$C$20*($B58+273)/6/PI()/C43/($C$26/1000000000)</f>
+        <v>2.0287790496937642E-19</v>
+      </c>
+      <c r="D58" s="7">
+        <f t="shared" si="10"/>
+        <v>2.4659279627516293E-19</v>
+      </c>
+      <c r="E58" s="7">
+        <f t="shared" si="10"/>
+        <v>3.240595448003212E-19</v>
+      </c>
+      <c r="F58" s="7">
+        <f t="shared" si="10"/>
+        <v>7.3545685801092863E-19</v>
+      </c>
+      <c r="G58" s="7">
+        <f t="shared" si="10"/>
+        <v>4.7875928580419481E-18</v>
+      </c>
+      <c r="H58" s="8">
+        <f t="shared" si="10"/>
+        <v>4.6043382385081698E-18</v>
+      </c>
+    </row>
+    <row r="59" spans="2:9">
+      <c r="B59" s="4">
+        <v>40</v>
+      </c>
+      <c r="C59" s="7">
+        <f t="shared" ref="C59:H59" si="11">$C$20*($B59+273)/6/PI()/C44/($C$26/1000000000)</f>
+        <v>2.5473117238985481E-19</v>
+      </c>
+      <c r="D59" s="7">
+        <f t="shared" si="11"/>
+        <v>2.7541039819960784E-19</v>
+      </c>
+      <c r="E59" s="7">
+        <f t="shared" si="11"/>
+        <v>6.4992429844872894E-19</v>
+      </c>
+      <c r="F59" s="7">
+        <f t="shared" si="11"/>
+        <v>1.2618210507331375E-18</v>
+      </c>
+      <c r="G59" s="7">
+        <f t="shared" si="11"/>
+        <v>6.2504850595115461E-18</v>
+      </c>
+      <c r="H59" s="8">
+        <f t="shared" si="11"/>
+        <v>5.7811580501479496E-18</v>
+      </c>
+    </row>
+    <row r="60" spans="2:9">
+      <c r="B60" s="4">
+        <v>50</v>
+      </c>
+      <c r="C60" s="7">
+        <f t="shared" ref="C60:H60" si="12">$C$20*($B60+273)/6/PI()/C45/($C$26/1000000000)</f>
+        <v>4.5397182681503085E-19</v>
+      </c>
+      <c r="D60" s="7">
+        <f t="shared" si="12"/>
+        <v>6.2033032619263806E-19</v>
+      </c>
+      <c r="E60" s="7">
+        <f t="shared" si="12"/>
+        <v>3.8835742526893167E-18</v>
+      </c>
+      <c r="F60" s="7">
+        <f t="shared" si="12"/>
+        <v>1.7111952815612779E-18</v>
+      </c>
+      <c r="G60" s="7">
+        <f t="shared" si="12"/>
+        <v>8.1520243700639029E-18</v>
+      </c>
+      <c r="H60" s="8">
+        <f t="shared" si="12"/>
+        <v>6.9738082779634628E-18</v>
+      </c>
+    </row>
+    <row r="61" spans="2:9">
+      <c r="B61" s="4">
+        <v>60</v>
+      </c>
+      <c r="C61" s="7">
+        <f t="shared" ref="C61:H61" si="13">$C$20*($B61+273)/6/PI()/C46/($C$26/1000000000)</f>
+        <v>1.2416497421787288E-18</v>
+      </c>
+      <c r="D61" s="7">
+        <f t="shared" si="13"/>
+        <v>1.2910650886745335E-18</v>
+      </c>
+      <c r="E61" s="7">
+        <f t="shared" si="13"/>
+        <v>1.8343851170305964E-18</v>
+      </c>
+      <c r="F61" s="7">
+        <f t="shared" si="13"/>
+        <v>4.501120836271861E-18</v>
+      </c>
+      <c r="G61" s="7">
+        <f t="shared" si="13"/>
+        <v>1.1484204712872389E-17</v>
+      </c>
+      <c r="H61" s="8">
+        <f t="shared" si="13"/>
+        <v>9.0866833191220391E-18</v>
+      </c>
+    </row>
+    <row r="62" spans="2:9">
+      <c r="B62" s="4">
+        <v>70</v>
+      </c>
+      <c r="C62" s="7">
+        <f t="shared" ref="C62:H62" si="14">$C$20*($B62+273)/6/PI()/C47/($C$26/1000000000)</f>
+        <v>2.7914630073393035E-17</v>
+      </c>
+      <c r="D62" s="7">
+        <f t="shared" si="14"/>
+        <v>3.0180756096634338E-18</v>
+      </c>
+      <c r="E62" s="7">
+        <f t="shared" si="14"/>
+        <v>4.4588385477566333E-18</v>
+      </c>
+      <c r="F62" s="7">
+        <f t="shared" si="14"/>
+        <v>2.5818656638010651E-17</v>
+      </c>
+      <c r="G62" s="7">
+        <f t="shared" si="14"/>
+        <v>3.1381936401568846E-16</v>
+      </c>
+      <c r="H62" s="8">
+        <f t="shared" si="14"/>
+        <v>1.7476012151831522E-16</v>
+      </c>
+    </row>
+    <row r="63" spans="2:9">
+      <c r="B63" s="4">
+        <v>80</v>
+      </c>
+      <c r="C63" s="7">
+        <f t="shared" ref="C63:H63" si="15">$C$20*($B63+273)/6/PI()/C48/($C$26/1000000000)</f>
+        <v>2.3635610710953753E-13</v>
+      </c>
+      <c r="D63" s="7">
+        <f t="shared" si="15"/>
+        <v>1.0015834810953401E-17</v>
+      </c>
+      <c r="E63" s="7">
+        <f t="shared" si="15"/>
+        <v>2.0219513622852318E-17</v>
+      </c>
+      <c r="F63" s="7">
+        <f t="shared" si="15"/>
+        <v>1.2658448868095901E-15</v>
+      </c>
+      <c r="G63" s="7">
+        <f t="shared" si="15"/>
+        <v>3.9255979961335654E-14</v>
+      </c>
+      <c r="H63" s="8">
+        <f t="shared" si="15"/>
+        <v>3.2296861661089804E-15</v>
+      </c>
+    </row>
+    <row r="64" spans="2:9" ht="15" thickBot="1">
+      <c r="B64" s="9">
+        <v>90</v>
+      </c>
+      <c r="C64" s="12">
+        <f t="shared" ref="C64:H64" si="16">$C$20*($B64+273)/6/PI()/C49/($C$26/1000000000)</f>
+        <v>1.1578846954316673E-12</v>
+      </c>
+      <c r="D64" s="12">
+        <f t="shared" si="16"/>
+        <v>5.3049659297780355E-16</v>
+      </c>
+      <c r="E64" s="12">
+        <f t="shared" si="16"/>
+        <v>6.7046657258904342E-16</v>
+      </c>
+      <c r="F64" s="12">
+        <f t="shared" si="16"/>
+        <v>1.5821890553323164E-12</v>
+      </c>
+      <c r="G64" s="12">
+        <f t="shared" si="16"/>
+        <v>1.2518817750068099E-11</v>
+      </c>
+      <c r="H64" s="13">
+        <f t="shared" si="16"/>
+        <v>7.8374377860703929E-12</v>
+      </c>
+    </row>
+    <row r="68" spans="3:3">
+      <c r="C68" s="14"/>
+    </row>
+    <row r="69" spans="3:3">
+      <c r="C69" s="14"/>
+    </row>
+    <row r="70" spans="3:3">
+      <c r="C70" s="14"/>
+    </row>
+    <row r="74" spans="3:3">
+      <c r="C74" s="14"/>
+    </row>
+    <row r="75" spans="3:3">
+      <c r="C75" s="14"/>
+    </row>
+    <row r="76" spans="3:3">
+      <c r="C76" s="14"/>
+    </row>
+    <row r="77" spans="3:3">
+      <c r="C77" s="14"/>
+    </row>
+    <row r="80" spans="3:3">
+      <c r="C80" s="14"/>
+    </row>
+    <row r="81" spans="3:3">
+      <c r="C81" s="14"/>
+    </row>
+    <row r="82" spans="3:3">
+      <c r="C82" s="14"/>
+    </row>
+    <row r="83" spans="3:3">
+      <c r="C83" s="14"/>
+    </row>
+    <row r="86" spans="3:3">
+      <c r="C86" s="14"/>
+    </row>
+    <row r="87" spans="3:3">
+      <c r="C87" s="14"/>
+    </row>
+    <row r="88" spans="3:3">
+      <c r="C88" s="14"/>
+    </row>
+    <row r="89" spans="3:3">
+      <c r="C89" s="14"/>
+    </row>
+    <row r="92" spans="3:3">
+      <c r="C92" s="14"/>
+    </row>
+    <row r="93" spans="3:3">
+      <c r="C93" s="14"/>
+    </row>
+    <row r="94" spans="3:3">
+      <c r="C94" s="14"/>
+    </row>
+    <row r="95" spans="3:3">
+      <c r="C95" s="14"/>
+    </row>
+    <row r="98" spans="3:3">
+      <c r="C98" s="14"/>
+    </row>
+    <row r="99" spans="3:3">
+      <c r="C99" s="14"/>
+    </row>
+    <row r="100" spans="3:3">
+      <c r="C100" s="14"/>
+    </row>
+    <row r="101" spans="3:3">
+      <c r="C101" s="14"/>
+    </row>
+    <row r="103" spans="3:3">
+      <c r="C103" s="14"/>
+    </row>
+    <row r="104" spans="3:3">
+      <c r="C104" s="14"/>
+    </row>
+    <row r="105" spans="3:3">
+      <c r="C105" s="14"/>
+    </row>
+    <row r="106" spans="3:3">
+      <c r="C106" s="14"/>
     </row>
   </sheetData>
+  <sortState ref="B39:H49">
+    <sortCondition ref="B39:B49"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
First draft versions of plots are ready
</commit_message>
<xml_diff>
--- a/Code/Timescale_Analysis/Equilibrium_Time_Data.xlsx
+++ b/Code/Timescale_Analysis/Equilibrium_Time_Data.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="120" windowWidth="18240" windowHeight="3150"/>
@@ -11,7 +11,7 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
@@ -181,8 +181,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="6">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -355,6 +355,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -420,6 +425,88 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>28575</xdr:colOff>
+          <xdr:row>23</xdr:row>
+          <xdr:rowOff>76200</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>5</xdr:col>
+          <xdr:colOff>695325</xdr:colOff>
+          <xdr:row>26</xdr:row>
+          <xdr:rowOff>38100</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1025" name="Object 1" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1025"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>8</xdr:col>
+          <xdr:colOff>171450</xdr:colOff>
+          <xdr:row>9</xdr:row>
+          <xdr:rowOff>171450</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>10</xdr:col>
+          <xdr:colOff>266700</xdr:colOff>
+          <xdr:row>15</xdr:row>
+          <xdr:rowOff>19050</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1026" name="Object 2" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1026"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
 </xdr:wsDr>
 </file>
 
@@ -498,6 +585,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -532,6 +620,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -707,20 +796,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:K106"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K50" sqref="K50"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="I49" sqref="I49"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="10.875" customWidth="1"/>
+    <col min="6" max="6" width="9.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:8" ht="15" thickBot="1"/>
-    <row r="2" spans="2:8" ht="16.5">
+    <row r="1" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="2:8" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B2" s="1" t="s">
         <v>17</v>
       </c>
@@ -731,7 +821,7 @@
       <c r="G2" s="2"/>
       <c r="H2" s="3"/>
     </row>
-    <row r="3" spans="2:8">
+    <row r="3" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B3" s="4"/>
       <c r="C3" s="5" t="s">
         <v>0</v>
@@ -742,7 +832,7 @@
       <c r="G3" s="5"/>
       <c r="H3" s="6"/>
     </row>
-    <row r="4" spans="2:8">
+    <row r="4" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B4" s="4" t="s">
         <v>1</v>
       </c>
@@ -765,7 +855,7 @@
         <v>0.95</v>
       </c>
     </row>
-    <row r="5" spans="2:8">
+    <row r="5" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B5" s="4">
         <v>1</v>
       </c>
@@ -788,7 +878,7 @@
         <v>6.9519300000000005E-7</v>
       </c>
     </row>
-    <row r="6" spans="2:8">
+    <row r="6" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B6" s="4">
         <v>10</v>
       </c>
@@ -811,7 +901,7 @@
         <v>7.2751499999999998E-4</v>
       </c>
     </row>
-    <row r="7" spans="2:8">
+    <row r="7" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B7" s="4">
         <v>100</v>
       </c>
@@ -834,7 +924,7 @@
         <v>4.34668E-2</v>
       </c>
     </row>
-    <row r="8" spans="2:8">
+    <row r="8" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B8" s="4">
         <v>1000</v>
       </c>
@@ -857,7 +947,7 @@
         <v>4.0911200000000001</v>
       </c>
     </row>
-    <row r="9" spans="2:8" ht="15" thickBot="1">
+    <row r="9" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B9" s="9">
         <v>10000</v>
       </c>
@@ -880,8 +970,8 @@
         <v>223.19499999999999</v>
       </c>
     </row>
-    <row r="10" spans="2:8" ht="15" thickBot="1"/>
-    <row r="11" spans="2:8" ht="15">
+    <row r="10" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="11" spans="2:8" ht="15" x14ac:dyDescent="0.25">
       <c r="B11" s="1" t="s">
         <v>11</v>
       </c>
@@ -892,7 +982,7 @@
       <c r="G11" s="2"/>
       <c r="H11" s="3"/>
     </row>
-    <row r="12" spans="2:8">
+    <row r="12" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B12" s="4"/>
       <c r="C12" s="5" t="s">
         <v>0</v>
@@ -903,7 +993,7 @@
       <c r="G12" s="5"/>
       <c r="H12" s="6"/>
     </row>
-    <row r="13" spans="2:8">
+    <row r="13" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B13" s="4" t="s">
         <v>1</v>
       </c>
@@ -926,7 +1016,7 @@
         <v>0.95</v>
       </c>
     </row>
-    <row r="14" spans="2:8">
+    <row r="14" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B14" s="4">
         <v>1</v>
       </c>
@@ -955,7 +1045,7 @@
         <v>1.0121208511155434E-17</v>
       </c>
     </row>
-    <row r="15" spans="2:8">
+    <row r="15" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B15" s="4">
         <v>10</v>
       </c>
@@ -984,7 +1074,7 @@
         <v>9.671543966097855E-19</v>
       </c>
     </row>
-    <row r="16" spans="2:8">
+    <row r="16" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B16" s="4">
         <v>100</v>
       </c>
@@ -1013,7 +1103,7 @@
         <v>1.6187511637607738E-18</v>
       </c>
     </row>
-    <row r="17" spans="2:11">
+    <row r="17" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B17" s="4">
         <v>1000</v>
       </c>
@@ -1049,7 +1139,7 @@
         <v>4.0171468013837419E-20</v>
       </c>
     </row>
-    <row r="18" spans="2:11" ht="15" thickBot="1">
+    <row r="18" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B18" s="9">
         <v>10000</v>
       </c>
@@ -1085,7 +1175,7 @@
         <v>1.1599605842663946E-17</v>
       </c>
     </row>
-    <row r="20" spans="2:11">
+    <row r="20" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B20" t="s">
         <v>2</v>
       </c>
@@ -1096,7 +1186,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="2:11">
+    <row r="21" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B21" t="s">
         <v>3</v>
       </c>
@@ -1107,12 +1197,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="23" spans="2:11" ht="16.5">
+    <row r="23" spans="2:11" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B23" s="15" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="24" spans="2:11" ht="28.5">
+    <row r="24" spans="2:11" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B24" s="16" t="s">
         <v>7</v>
       </c>
@@ -1121,7 +1211,7 @@
         <v>7500000</v>
       </c>
     </row>
-    <row r="25" spans="2:11">
+    <row r="25" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B25" t="s">
         <v>6</v>
       </c>
@@ -1130,7 +1220,7 @@
         <v>1.3702874892636524E-19</v>
       </c>
     </row>
-    <row r="26" spans="2:11" ht="16.5">
+    <row r="26" spans="2:11" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B26" s="17" t="s">
         <v>9</v>
       </c>
@@ -1139,12 +1229,12 @@
         <v>0.21228595964934563</v>
       </c>
     </row>
-    <row r="28" spans="2:11" ht="15">
+    <row r="28" spans="2:11" ht="15" x14ac:dyDescent="0.25">
       <c r="B28" s="15" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="30" spans="2:11">
+    <row r="30" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B30" t="s">
         <v>8</v>
       </c>
@@ -1164,7 +1254,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="31" spans="2:11" ht="28.5">
+    <row r="31" spans="2:11" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B31" s="16" t="s">
         <v>7</v>
       </c>
@@ -1184,7 +1274,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="32" spans="2:11">
+    <row r="32" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B32" t="s">
         <v>6</v>
       </c>
@@ -1209,8 +1299,8 @@
         <v>1.4588043824459524E-10</v>
       </c>
     </row>
-    <row r="35" spans="2:8" ht="15" thickBot="1"/>
-    <row r="36" spans="2:8" ht="15">
+    <row r="35" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="36" spans="2:8" ht="15" x14ac:dyDescent="0.25">
       <c r="B36" s="1" t="s">
         <v>16</v>
       </c>
@@ -1221,7 +1311,7 @@
       <c r="G36" s="2"/>
       <c r="H36" s="3"/>
     </row>
-    <row r="37" spans="2:8">
+    <row r="37" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B37" s="4"/>
       <c r="C37" s="5" t="s">
         <v>14</v>
@@ -1232,7 +1322,7 @@
       <c r="G37" s="5"/>
       <c r="H37" s="6"/>
     </row>
-    <row r="38" spans="2:8">
+    <row r="38" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B38" s="4" t="s">
         <v>15</v>
       </c>
@@ -1255,7 +1345,7 @@
         <v>0.95</v>
       </c>
     </row>
-    <row r="39" spans="2:8">
+    <row r="39" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B39" s="4">
         <v>0</v>
       </c>
@@ -1263,13 +1353,13 @@
         <v>8554670</v>
       </c>
       <c r="D39" s="7">
-        <v>5568810</v>
+        <v>8554670</v>
       </c>
       <c r="E39" s="7">
         <v>8554670</v>
       </c>
       <c r="F39" s="7">
-        <v>1867180</v>
+        <v>1941490</v>
       </c>
       <c r="G39" s="5">
         <v>275853</v>
@@ -1278,7 +1368,7 @@
         <v>286832</v>
       </c>
     </row>
-    <row r="40" spans="2:8">
+    <row r="40" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B40" s="4">
         <v>5</v>
       </c>
@@ -1286,22 +1376,22 @@
         <v>8227240</v>
       </c>
       <c r="D40" s="7">
-        <v>5568810</v>
+        <v>7609500</v>
       </c>
       <c r="E40" s="7">
         <v>7609500</v>
       </c>
       <c r="F40" s="7">
-        <v>1941490</v>
+        <v>1867180</v>
       </c>
       <c r="G40" s="5">
-        <v>255141</v>
+        <v>260000</v>
       </c>
       <c r="H40" s="6">
         <v>286832</v>
       </c>
     </row>
-    <row r="41" spans="2:8">
+    <row r="41" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B41" s="4">
         <v>10</v>
       </c>
@@ -1309,7 +1399,7 @@
         <v>7318240</v>
       </c>
       <c r="D41" s="7">
-        <v>5568810</v>
+        <v>7038140</v>
       </c>
       <c r="E41" s="7">
         <v>7038140</v>
@@ -1324,7 +1414,7 @@
         <v>275853</v>
       </c>
     </row>
-    <row r="42" spans="2:8">
+    <row r="42" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B42" s="4">
         <v>20</v>
       </c>
@@ -1332,7 +1422,7 @@
         <v>5355670</v>
       </c>
       <c r="D42" s="7">
-        <v>4406240</v>
+        <v>4953540</v>
       </c>
       <c r="E42" s="7">
         <v>4953540</v>
@@ -1347,7 +1437,7 @@
         <v>265295</v>
       </c>
     </row>
-    <row r="43" spans="2:8">
+    <row r="43" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B43" s="4">
         <v>30</v>
       </c>
@@ -1370,7 +1460,7 @@
         <v>226951</v>
       </c>
     </row>
-    <row r="44" spans="2:8">
+    <row r="44" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B44" s="4">
         <v>40</v>
       </c>
@@ -1393,7 +1483,7 @@
         <v>186718</v>
       </c>
     </row>
-    <row r="45" spans="2:8">
+    <row r="45" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B45" s="4">
         <v>50</v>
       </c>
@@ -1404,7 +1494,7 @@
         <v>1795710</v>
       </c>
       <c r="E45" s="5">
-        <v>286832</v>
+        <v>626052</v>
       </c>
       <c r="F45" s="5">
         <v>650968</v>
@@ -1416,7 +1506,7 @@
         <v>159731</v>
       </c>
     </row>
-    <row r="46" spans="2:8">
+    <row r="46" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B46" s="4">
         <v>60</v>
       </c>
@@ -1427,7 +1517,7 @@
         <v>889514</v>
       </c>
       <c r="E46" s="5">
-        <v>626052</v>
+        <v>286832</v>
       </c>
       <c r="F46" s="5">
         <v>255141</v>
@@ -1439,7 +1529,7 @@
         <v>126385</v>
       </c>
     </row>
-    <row r="47" spans="2:8">
+    <row r="47" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B47" s="4">
         <v>70</v>
       </c>
@@ -1462,12 +1552,12 @@
         <v>6768.75</v>
       </c>
     </row>
-    <row r="48" spans="2:8">
+    <row r="48" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B48" s="4">
         <v>80</v>
       </c>
       <c r="C48" s="5">
-        <v>5.1506800000000004</v>
+        <v>121547</v>
       </c>
       <c r="D48" s="5">
         <v>121547</v>
@@ -1485,12 +1575,12 @@
         <v>376.93900000000002</v>
       </c>
     </row>
-    <row r="49" spans="2:9" ht="15" thickBot="1">
+    <row r="49" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B49" s="9">
         <v>90</v>
       </c>
       <c r="C49" s="10">
-        <v>1.08118</v>
+        <v>2359.83</v>
       </c>
       <c r="D49" s="10">
         <v>2359.83</v>
@@ -1508,14 +1598,14 @@
         <v>0.15973100000000001</v>
       </c>
     </row>
-    <row r="50" spans="2:9" ht="15" thickBot="1">
+    <row r="50" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B50" s="14"/>
       <c r="F50" s="14"/>
       <c r="G50" s="14"/>
       <c r="H50" s="14"/>
       <c r="I50" s="14"/>
     </row>
-    <row r="51" spans="2:9" ht="15">
+    <row r="51" spans="2:9" ht="15" x14ac:dyDescent="0.25">
       <c r="B51" s="1" t="s">
         <v>18</v>
       </c>
@@ -1526,7 +1616,7 @@
       <c r="G51" s="2"/>
       <c r="H51" s="3"/>
     </row>
-    <row r="52" spans="2:9">
+    <row r="52" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B52" s="4"/>
       <c r="C52" s="5" t="s">
         <v>14</v>
@@ -1537,7 +1627,7 @@
       <c r="G52" s="5"/>
       <c r="H52" s="6"/>
     </row>
-    <row r="53" spans="2:9">
+    <row r="53" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B53" s="4" t="s">
         <v>15</v>
       </c>
@@ -1560,7 +1650,7 @@
         <v>0.95</v>
       </c>
     </row>
-    <row r="54" spans="2:9">
+    <row r="54" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B54" s="4">
         <v>0</v>
       </c>
@@ -1570,26 +1660,26 @@
       </c>
       <c r="D54" s="7">
         <f t="shared" ref="D54:H54" si="6">$C$20*($B54+273)/6/PI()/D39/($C$26/1000000000)</f>
-        <v>1.6906625721619102E-19</v>
+        <v>1.1005659643774648E-19</v>
       </c>
       <c r="E54" s="7">
         <f t="shared" si="6"/>
         <v>1.1005659643774648E-19</v>
       </c>
       <c r="F54" s="7">
-        <f t="shared" si="6"/>
+        <f>$C$20*($B54+273)/6/PI()/F40/($C$26/1000000000)</f>
         <v>5.0423519095539618E-19</v>
       </c>
       <c r="G54" s="7">
         <f t="shared" si="6"/>
         <v>3.4130419602037921E-18</v>
       </c>
-      <c r="H54" s="8">
+      <c r="H54" s="7">
         <f t="shared" si="6"/>
         <v>3.2824017677528889E-18</v>
       </c>
     </row>
-    <row r="55" spans="2:9">
+    <row r="55" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B55" s="4">
         <v>5</v>
       </c>
@@ -1598,366 +1688,366 @@
         <v>1.1653256918091916E-19</v>
       </c>
       <c r="D55" s="7">
-        <f t="shared" si="7"/>
-        <v>1.7216270881355716E-19</v>
+        <f t="shared" ref="D55:H55" si="8">$C$20*($B55+273)/6/PI()/D40/($C$26/1000000000)</f>
+        <v>1.2599269524515739E-19</v>
       </c>
       <c r="E55" s="7">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1.2599269524515739E-19</v>
       </c>
       <c r="F55" s="7">
-        <f t="shared" si="7"/>
+        <f>$C$20*($B55+273)/6/PI()/F39/($C$26/1000000000)</f>
         <v>4.9381733332029787E-19</v>
       </c>
       <c r="G55" s="7">
-        <f t="shared" si="7"/>
-        <v>3.7576924699206523E-18</v>
-      </c>
-      <c r="H55" s="8">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
+        <v>3.6874669787231739E-18</v>
+      </c>
+      <c r="H55" s="7">
+        <f t="shared" si="8"/>
         <v>3.3425190162465315E-18</v>
       </c>
     </row>
-    <row r="56" spans="2:9">
+    <row r="56" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B56" s="4">
         <v>10</v>
       </c>
       <c r="C56" s="7">
-        <f t="shared" ref="C56:H56" si="8">$C$20*($B56+273)/6/PI()/C41/($C$26/1000000000)</f>
+        <f t="shared" ref="C56:H56" si="9">$C$20*($B56+273)/6/PI()/C41/($C$26/1000000000)</f>
         <v>1.3336334488728904E-19</v>
       </c>
       <c r="D56" s="7">
-        <f t="shared" si="8"/>
-        <v>1.7525916041092333E-19</v>
+        <f t="shared" ref="D56:H56" si="10">$C$20*($B56+273)/6/PI()/D41/($C$26/1000000000)</f>
+        <v>1.3867086546842689E-19</v>
       </c>
       <c r="E56" s="7">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>1.3867086546842689E-19</v>
       </c>
       <c r="F56" s="7">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>5.4350923316568599E-19</v>
       </c>
       <c r="G56" s="7">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>3.8252768668616721E-18</v>
       </c>
-      <c r="H56" s="8">
-        <f t="shared" si="8"/>
+      <c r="H56" s="7">
+        <f t="shared" si="10"/>
         <v>3.5380618122259101E-18</v>
       </c>
     </row>
-    <row r="57" spans="2:9">
+    <row r="57" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B57" s="4">
         <v>20</v>
       </c>
       <c r="C57" s="7">
-        <f t="shared" ref="C57:H57" si="9">$C$20*($B57+273)/6/PI()/C42/($C$26/1000000000)</f>
+        <f t="shared" ref="C57:H57" si="11">$C$20*($B57+273)/6/PI()/C42/($C$26/1000000000)</f>
         <v>1.8867332496733574E-19</v>
       </c>
       <c r="D57" s="7">
-        <f t="shared" si="9"/>
-        <v>2.2932751423613125E-19</v>
+        <f t="shared" ref="D57:H57" si="12">$C$20*($B57+273)/6/PI()/D42/($C$26/1000000000)</f>
+        <v>2.0398988729833835E-19</v>
       </c>
       <c r="E57" s="7">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>2.0398988729833835E-19</v>
       </c>
       <c r="F57" s="7">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>6.57782334314866E-19</v>
       </c>
       <c r="G57" s="7">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>4.4523798808016312E-18</v>
       </c>
-      <c r="H57" s="8">
-        <f t="shared" si="9"/>
+      <c r="H57" s="7">
+        <f t="shared" si="12"/>
         <v>3.808862083069077E-18</v>
       </c>
     </row>
-    <row r="58" spans="2:9">
+    <row r="58" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B58" s="4">
         <v>30</v>
       </c>
       <c r="C58" s="7">
-        <f t="shared" ref="C58:H58" si="10">$C$20*($B58+273)/6/PI()/C43/($C$26/1000000000)</f>
+        <f t="shared" ref="C58:H58" si="13">$C$20*($B58+273)/6/PI()/C43/($C$26/1000000000)</f>
         <v>2.0287790496937642E-19</v>
       </c>
       <c r="D58" s="7">
-        <f t="shared" si="10"/>
+        <f t="shared" ref="D58:H58" si="14">$C$20*($B58+273)/6/PI()/D43/($C$26/1000000000)</f>
         <v>2.4659279627516293E-19</v>
       </c>
       <c r="E58" s="7">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>3.240595448003212E-19</v>
       </c>
       <c r="F58" s="7">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>7.3545685801092863E-19</v>
       </c>
       <c r="G58" s="7">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>4.7875928580419481E-18</v>
       </c>
-      <c r="H58" s="8">
-        <f t="shared" si="10"/>
+      <c r="H58" s="7">
+        <f t="shared" si="14"/>
         <v>4.6043382385081698E-18</v>
       </c>
     </row>
-    <row r="59" spans="2:9">
+    <row r="59" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B59" s="4">
         <v>40</v>
       </c>
       <c r="C59" s="7">
-        <f t="shared" ref="C59:H59" si="11">$C$20*($B59+273)/6/PI()/C44/($C$26/1000000000)</f>
+        <f t="shared" ref="C59:H59" si="15">$C$20*($B59+273)/6/PI()/C44/($C$26/1000000000)</f>
         <v>2.5473117238985481E-19</v>
       </c>
       <c r="D59" s="7">
-        <f t="shared" si="11"/>
+        <f t="shared" ref="D59:H59" si="16">$C$20*($B59+273)/6/PI()/D44/($C$26/1000000000)</f>
         <v>2.7541039819960784E-19</v>
       </c>
       <c r="E59" s="7">
-        <f t="shared" si="11"/>
+        <f t="shared" si="16"/>
         <v>6.4992429844872894E-19</v>
       </c>
       <c r="F59" s="7">
-        <f t="shared" si="11"/>
+        <f t="shared" si="16"/>
         <v>1.2618210507331375E-18</v>
       </c>
       <c r="G59" s="7">
-        <f t="shared" si="11"/>
+        <f t="shared" si="16"/>
         <v>6.2504850595115461E-18</v>
       </c>
-      <c r="H59" s="8">
-        <f t="shared" si="11"/>
+      <c r="H59" s="7">
+        <f t="shared" si="16"/>
         <v>5.7811580501479496E-18</v>
       </c>
     </row>
-    <row r="60" spans="2:9">
+    <row r="60" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B60" s="4">
         <v>50</v>
       </c>
       <c r="C60" s="7">
-        <f t="shared" ref="C60:H60" si="12">$C$20*($B60+273)/6/PI()/C45/($C$26/1000000000)</f>
+        <f t="shared" ref="C60:H60" si="17">$C$20*($B60+273)/6/PI()/C45/($C$26/1000000000)</f>
         <v>4.5397182681503085E-19</v>
       </c>
       <c r="D60" s="7">
-        <f t="shared" si="12"/>
+        <f t="shared" ref="D60:H60" si="18">$C$20*($B60+273)/6/PI()/D45/($C$26/1000000000)</f>
         <v>6.2033032619263806E-19</v>
       </c>
       <c r="E60" s="7">
-        <f t="shared" si="12"/>
-        <v>3.8835742526893167E-18</v>
+        <f t="shared" si="18"/>
+        <v>1.7792984768795274E-18</v>
       </c>
       <c r="F60" s="7">
-        <f t="shared" si="12"/>
+        <f t="shared" si="18"/>
         <v>1.7111952815612779E-18</v>
       </c>
       <c r="G60" s="7">
-        <f t="shared" si="12"/>
+        <f t="shared" si="18"/>
         <v>8.1520243700639029E-18</v>
       </c>
-      <c r="H60" s="8">
-        <f t="shared" si="12"/>
+      <c r="H60" s="7">
+        <f t="shared" si="18"/>
         <v>6.9738082779634628E-18</v>
       </c>
     </row>
-    <row r="61" spans="2:9">
+    <row r="61" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B61" s="4">
         <v>60</v>
       </c>
       <c r="C61" s="7">
-        <f t="shared" ref="C61:H61" si="13">$C$20*($B61+273)/6/PI()/C46/($C$26/1000000000)</f>
+        <f t="shared" ref="C61:H61" si="19">$C$20*($B61+273)/6/PI()/C46/($C$26/1000000000)</f>
         <v>1.2416497421787288E-18</v>
       </c>
       <c r="D61" s="7">
-        <f t="shared" si="13"/>
+        <f t="shared" ref="D61:H61" si="20">$C$20*($B61+273)/6/PI()/D46/($C$26/1000000000)</f>
         <v>1.2910650886745335E-18</v>
       </c>
       <c r="E61" s="7">
-        <f t="shared" si="13"/>
-        <v>1.8343851170305964E-18</v>
+        <f t="shared" si="20"/>
+        <v>4.0038087496766011E-18</v>
       </c>
       <c r="F61" s="7">
-        <f t="shared" si="13"/>
+        <f t="shared" si="20"/>
         <v>4.501120836271861E-18</v>
       </c>
       <c r="G61" s="7">
-        <f t="shared" si="13"/>
+        <f t="shared" si="20"/>
         <v>1.1484204712872389E-17</v>
       </c>
-      <c r="H61" s="8">
-        <f t="shared" si="13"/>
+      <c r="H61" s="7">
+        <f t="shared" si="20"/>
         <v>9.0866833191220391E-18</v>
       </c>
     </row>
-    <row r="62" spans="2:9">
+    <row r="62" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B62" s="4">
         <v>70</v>
       </c>
       <c r="C62" s="7">
-        <f t="shared" ref="C62:H62" si="14">$C$20*($B62+273)/6/PI()/C47/($C$26/1000000000)</f>
+        <f t="shared" ref="C62:H62" si="21">$C$20*($B62+273)/6/PI()/C47/($C$26/1000000000)</f>
         <v>2.7914630073393035E-17</v>
       </c>
       <c r="D62" s="7">
-        <f t="shared" si="14"/>
+        <f t="shared" ref="D62:H62" si="22">$C$20*($B62+273)/6/PI()/D47/($C$26/1000000000)</f>
         <v>3.0180756096634338E-18</v>
       </c>
       <c r="E62" s="7">
-        <f t="shared" si="14"/>
+        <f t="shared" si="22"/>
         <v>4.4588385477566333E-18</v>
       </c>
       <c r="F62" s="7">
-        <f t="shared" si="14"/>
+        <f t="shared" si="22"/>
         <v>2.5818656638010651E-17</v>
       </c>
       <c r="G62" s="7">
-        <f t="shared" si="14"/>
+        <f t="shared" si="22"/>
         <v>3.1381936401568846E-16</v>
       </c>
-      <c r="H62" s="8">
-        <f t="shared" si="14"/>
+      <c r="H62" s="7">
+        <f t="shared" si="22"/>
         <v>1.7476012151831522E-16</v>
       </c>
     </row>
-    <row r="63" spans="2:9">
+    <row r="63" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B63" s="4">
         <v>80</v>
       </c>
       <c r="C63" s="7">
-        <f t="shared" ref="C63:H63" si="15">$C$20*($B63+273)/6/PI()/C48/($C$26/1000000000)</f>
-        <v>2.3635610710953753E-13</v>
+        <f t="shared" ref="C63:H63" si="23">$C$20*($B63+273)/6/PI()/C48/($C$26/1000000000)</f>
+        <v>1.0015834810953401E-17</v>
       </c>
       <c r="D63" s="7">
-        <f t="shared" si="15"/>
+        <f t="shared" ref="D63:H63" si="24">$C$20*($B63+273)/6/PI()/D48/($C$26/1000000000)</f>
         <v>1.0015834810953401E-17</v>
       </c>
       <c r="E63" s="7">
-        <f t="shared" si="15"/>
+        <f t="shared" si="24"/>
         <v>2.0219513622852318E-17</v>
       </c>
       <c r="F63" s="7">
-        <f t="shared" si="15"/>
+        <f t="shared" si="24"/>
         <v>1.2658448868095901E-15</v>
       </c>
       <c r="G63" s="7">
-        <f t="shared" si="15"/>
+        <f t="shared" si="24"/>
         <v>3.9255979961335654E-14</v>
       </c>
-      <c r="H63" s="8">
-        <f t="shared" si="15"/>
+      <c r="H63" s="7">
+        <f t="shared" si="24"/>
         <v>3.2296861661089804E-15</v>
       </c>
     </row>
-    <row r="64" spans="2:9" ht="15" thickBot="1">
+    <row r="64" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B64" s="9">
         <v>90</v>
       </c>
-      <c r="C64" s="12">
-        <f t="shared" ref="C64:H64" si="16">$C$20*($B64+273)/6/PI()/C49/($C$26/1000000000)</f>
-        <v>1.1578846954316673E-12</v>
-      </c>
-      <c r="D64" s="12">
-        <f t="shared" si="16"/>
+      <c r="C64" s="7">
+        <f t="shared" ref="C64:H64" si="25">$C$20*($B64+273)/6/PI()/C49/($C$26/1000000000)</f>
         <v>5.3049659297780355E-16</v>
       </c>
-      <c r="E64" s="12">
-        <f t="shared" si="16"/>
+      <c r="D64" s="7">
+        <f t="shared" ref="D64:H64" si="26">$C$20*($B64+273)/6/PI()/D49/($C$26/1000000000)</f>
+        <v>5.3049659297780355E-16</v>
+      </c>
+      <c r="E64" s="7">
+        <f t="shared" si="26"/>
         <v>6.7046657258904342E-16</v>
       </c>
-      <c r="F64" s="12">
-        <f t="shared" si="16"/>
+      <c r="F64" s="7">
+        <f t="shared" si="26"/>
         <v>1.5821890553323164E-12</v>
       </c>
-      <c r="G64" s="12">
-        <f t="shared" si="16"/>
+      <c r="G64" s="7">
+        <f t="shared" si="26"/>
         <v>1.2518817750068099E-11</v>
       </c>
-      <c r="H64" s="13">
-        <f t="shared" si="16"/>
+      <c r="H64" s="7">
+        <f t="shared" si="26"/>
         <v>7.8374377860703929E-12</v>
       </c>
     </row>
-    <row r="68" spans="3:3">
+    <row r="68" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C68" s="14"/>
     </row>
-    <row r="69" spans="3:3">
+    <row r="69" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C69" s="14"/>
     </row>
-    <row r="70" spans="3:3">
+    <row r="70" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C70" s="14"/>
     </row>
-    <row r="74" spans="3:3">
+    <row r="74" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C74" s="14"/>
     </row>
-    <row r="75" spans="3:3">
+    <row r="75" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C75" s="14"/>
     </row>
-    <row r="76" spans="3:3">
+    <row r="76" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C76" s="14"/>
     </row>
-    <row r="77" spans="3:3">
+    <row r="77" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C77" s="14"/>
     </row>
-    <row r="80" spans="3:3">
+    <row r="80" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C80" s="14"/>
     </row>
-    <row r="81" spans="3:3">
+    <row r="81" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C81" s="14"/>
     </row>
-    <row r="82" spans="3:3">
+    <row r="82" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C82" s="14"/>
     </row>
-    <row r="83" spans="3:3">
+    <row r="83" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C83" s="14"/>
     </row>
-    <row r="86" spans="3:3">
+    <row r="86" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C86" s="14"/>
     </row>
-    <row r="87" spans="3:3">
+    <row r="87" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C87" s="14"/>
     </row>
-    <row r="88" spans="3:3">
+    <row r="88" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C88" s="14"/>
     </row>
-    <row r="89" spans="3:3">
+    <row r="89" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C89" s="14"/>
     </row>
-    <row r="92" spans="3:3">
+    <row r="92" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C92" s="14"/>
     </row>
-    <row r="93" spans="3:3">
+    <row r="93" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C93" s="14"/>
     </row>
-    <row r="94" spans="3:3">
+    <row r="94" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C94" s="14"/>
     </row>
-    <row r="95" spans="3:3">
+    <row r="95" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C95" s="14"/>
     </row>
-    <row r="98" spans="3:3">
+    <row r="98" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C98" s="14"/>
     </row>
-    <row r="99" spans="3:3">
+    <row r="99" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C99" s="14"/>
     </row>
-    <row r="100" spans="3:3">
+    <row r="100" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C100" s="14"/>
     </row>
-    <row r="101" spans="3:3">
+    <row r="101" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C101" s="14"/>
     </row>
-    <row r="103" spans="3:3">
+    <row r="103" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C103" s="14"/>
     </row>
-    <row r="104" spans="3:3">
+    <row r="104" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C104" s="14"/>
     </row>
-    <row r="105" spans="3:3">
+    <row r="105" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C105" s="14"/>
     </row>
-    <row r="106" spans="3:3">
+    <row r="106" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C106" s="14"/>
     </row>
   </sheetData>
@@ -1969,31 +2059,79 @@
   <drawing r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
   <oleObjects>
-    <oleObject progId="Equation.3" shapeId="1025" r:id="rId3"/>
-    <oleObject progId="Equation.3" shapeId="1026" r:id="rId4"/>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <oleObject progId="Equation.3" shapeId="1025" r:id="rId3">
+          <objectPr defaultSize="0" autoPict="0" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>28575</xdr:colOff>
+                <xdr:row>23</xdr:row>
+                <xdr:rowOff>76200</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>695325</xdr:colOff>
+                <xdr:row>26</xdr:row>
+                <xdr:rowOff>38100</xdr:rowOff>
+              </to>
+            </anchor>
+          </objectPr>
+        </oleObject>
+      </mc:Choice>
+      <mc:Fallback>
+        <oleObject progId="Equation.3" shapeId="1025" r:id="rId3"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <oleObject progId="Equation.3" shapeId="1026" r:id="rId5">
+          <objectPr defaultSize="0" autoPict="0" r:id="rId6">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>8</xdr:col>
+                <xdr:colOff>171450</xdr:colOff>
+                <xdr:row>9</xdr:row>
+                <xdr:rowOff>171450</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>10</xdr:col>
+                <xdr:colOff>266700</xdr:colOff>
+                <xdr:row>15</xdr:row>
+                <xdr:rowOff>19050</xdr:rowOff>
+              </to>
+            </anchor>
+          </objectPr>
+        </oleObject>
+      </mc:Choice>
+      <mc:Fallback>
+        <oleObject progId="Equation.3" shapeId="1026" r:id="rId5"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
   </oleObjects>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>